<commit_message>
corrected module type and added 2 new N number for new module arm and mim
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_EWH/WG_Number_excel_table.xlsx
+++ b/publication/part1000/CR_EWH/WG_Number_excel_table.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klt/Projets/EclipseWS/stepmod/publication/part1000/CR_210_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klt/Projets/EclipseWS/stepmod/publication/part1000/CR_EWH/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="200" yWindow="460" windowWidth="26940" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="6580" yWindow="-19700" windowWidth="28800" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WG NB" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="104">
   <si>
     <t>Submitter</t>
   </si>
@@ -39,13 +39,316 @@
   </si>
   <si>
     <t>N#</t>
+  </si>
+  <si>
+    <t>ISO 10303-1636 ed5 assembly_module_design Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1636 ed5 assembly_module_design ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1636 ed5 assembly_module_design MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1642 ed5 assembly_module_usage_view Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1642 ed5 assembly_module_usage_view ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1642 ed5 assembly_module_usage_view MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1649 ed4 assembly_technology Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1649 ed4 assembly_technology ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1649 ed4 assembly_technology MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1653 ed4 cable Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1653 ed4 cable ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1653 ed4 cable MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1657 ed4 component_feature Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1657 ed4 component_feature ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1657 ed4 component_feature MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1674 ed3 functional_assignment_to_part Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1674 ed3 functional_assignment_to_part ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1674 ed3 functional_assignment_to_part MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1679 ed3 functional_specification Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1679 ed3 functional_specification ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1679 ed3 functional_specification MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1691 ed4 interface_component Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1691 ed4 interface_component ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1703 ed5 model_parameter Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1703 ed5 model_parameter ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1703 ed5 model_parameter MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1704 ed4 network_functional_design_view Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1704 ed4 network_functional_design_view ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1704 ed4 network_functional_design_view MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1705 ed5 functional_usage_view Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1705 ed5 functional_usage_view ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1705 ed5 functional_usage_view MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1714 ed4 part_feature_location Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1714 ed4 part_feature_location ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1714 ed4 part_feature_location MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1721 ed4 physical_component_feature Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1721 ed4 physical_component_feature ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1732 ed5 physical_unit_usage_view Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1732 ed5 physical_unit_usage_view ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1732 ed5 physical_unit_usage_view MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>N9475</t>
+  </si>
+  <si>
+    <t>N9476</t>
+  </si>
+  <si>
+    <t>N9477</t>
+  </si>
+  <si>
+    <t>N9478</t>
+  </si>
+  <si>
+    <t>N9479</t>
+  </si>
+  <si>
+    <t>N9480</t>
+  </si>
+  <si>
+    <t>N9481</t>
+  </si>
+  <si>
+    <t>N9482</t>
+  </si>
+  <si>
+    <t>N9483</t>
+  </si>
+  <si>
+    <t>N9484</t>
+  </si>
+  <si>
+    <t>N9485</t>
+  </si>
+  <si>
+    <t>N9486</t>
+  </si>
+  <si>
+    <t>N9487</t>
+  </si>
+  <si>
+    <t>N9488</t>
+  </si>
+  <si>
+    <t>N9489</t>
+  </si>
+  <si>
+    <t>N9490</t>
+  </si>
+  <si>
+    <t>N9491</t>
+  </si>
+  <si>
+    <t>N9492</t>
+  </si>
+  <si>
+    <t>N9493</t>
+  </si>
+  <si>
+    <t>N9494</t>
+  </si>
+  <si>
+    <t>N9495</t>
+  </si>
+  <si>
+    <t>N9496</t>
+  </si>
+  <si>
+    <t>N9497</t>
+  </si>
+  <si>
+    <t>N9498</t>
+  </si>
+  <si>
+    <t>N9499</t>
+  </si>
+  <si>
+    <t>N9500</t>
+  </si>
+  <si>
+    <t>N9501</t>
+  </si>
+  <si>
+    <t>N9502</t>
+  </si>
+  <si>
+    <t>N9503</t>
+  </si>
+  <si>
+    <t>N9504</t>
+  </si>
+  <si>
+    <t>N9505</t>
+  </si>
+  <si>
+    <t>N9506</t>
+  </si>
+  <si>
+    <t>N9507</t>
+  </si>
+  <si>
+    <t>N9508</t>
+  </si>
+  <si>
+    <t>N9509</t>
+  </si>
+  <si>
+    <t>N9510</t>
+  </si>
+  <si>
+    <t>N9511</t>
+  </si>
+  <si>
+    <t>N9512</t>
+  </si>
+  <si>
+    <t>N9513</t>
+  </si>
+  <si>
+    <t>N9514</t>
+  </si>
+  <si>
+    <t>N9515</t>
+  </si>
+  <si>
+    <t>N9516</t>
+  </si>
+  <si>
+    <t>N9517</t>
+  </si>
+  <si>
+    <t>N9518</t>
+  </si>
+  <si>
+    <t>N9519</t>
+  </si>
+  <si>
+    <t>N9520</t>
+  </si>
+  <si>
+    <t>N9521</t>
+  </si>
+  <si>
+    <t>Aminata Mbengue</t>
+  </si>
+  <si>
+    <t>ISO 10303-1740 ed4 requirement_decomposition Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1740 ed4 requirement_decomposition ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1740 ed4 requirement_decomposition MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1755 ed5 physical_connectivity_definition Document</t>
+  </si>
+  <si>
+    <t>ISO 10303-1755 ed5 physical_connectivity_definition ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1755 ed5 physical_connectivity_definition MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1827 ed1 extruded_structure_cross_section Document</t>
+  </si>
+  <si>
+    <t>modified</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>ISO 10303-1827 ed1 extruded_structure_cross_section ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>ISO 10303-1827 ed1 extruded_structure_cross_section MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -71,6 +374,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Monaco"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Cambria"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -80,7 +399,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -103,13 +422,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -121,6 +451,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -402,15 +741,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="92.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" customWidth="1"/>
@@ -433,308 +772,793 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
+      <c r="E4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
+      <c r="E6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
+      <c r="E7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
+      <c r="E8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
+      <c r="E9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
+      <c r="E10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
+      <c r="E11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
+      <c r="E12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
+      <c r="E13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
+      <c r="E14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
+      <c r="E15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
+      <c r="E16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
+      <c r="E17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
+      <c r="E18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
+      <c r="E19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
+      <c r="E20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="4"/>
+      <c r="E21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
+      <c r="E22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+      <c r="A23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
+      <c r="E23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+      <c r="A24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
+      <c r="E24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+      <c r="A25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="4"/>
+      <c r="E25" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+      <c r="A26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
+      <c r="E26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+      <c r="A27" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
+      <c r="E27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="A28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
+      <c r="E28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
+      <c r="E29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+      <c r="A30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
+      <c r="E30" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+      <c r="A31" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="4"/>
+      <c r="E31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="6">
+        <v>42796</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
+      <c r="A32" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+      <c r="E32" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+      <c r="E33" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
+      <c r="E34" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
+      <c r="E35" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
+      <c r="E36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="4"/>
-    </row>
-    <row r="38" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
+      <c r="E37" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="4"/>
-    </row>
-    <row r="39" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
+      <c r="E38" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="4"/>
+      <c r="E39" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F42" s="6">
+        <v>42796</v>
+      </c>
+      <c r="G42" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F43" s="6">
+        <v>42796</v>
+      </c>
+      <c r="G43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F44" s="6">
+        <v>42796</v>
+      </c>
+      <c r="G44" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F45" s="6">
+        <v>42796</v>
+      </c>
+      <c r="G45" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F46" s="6">
+        <v>42796</v>
+      </c>
+      <c r="G46" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F47" s="6">
+        <v>42796</v>
+      </c>
+      <c r="G47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F48" s="6">
+        <v>42796</v>
+      </c>
+      <c r="G48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F49" s="7">
+        <v>42811</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F50" s="7">
+        <v>42811</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added missing WG Number for new module
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_EWH/WG_Number_excel_table.xlsx
+++ b/publication/part1000/CR_EWH/WG_Number_excel_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="-18200" windowWidth="28800" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="10120" yWindow="-19280" windowWidth="28800" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WG NB" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="103">
   <si>
     <t>Submitter</t>
   </si>
@@ -326,19 +326,16 @@
     <t>ISO 10303-1827 ed1 extruded_structure_cross_section Document</t>
   </si>
   <si>
-    <t>modified</t>
-  </si>
-  <si>
-    <t>new</t>
-  </si>
-  <si>
     <t>ISO 10303-1827 ed1 extruded_structure_cross_section ARM EXPRESS</t>
   </si>
   <si>
     <t>ISO 10303-1827 ed1 extruded_structure_cross_section MIM EXPRESS</t>
   </si>
   <si>
-    <t>N</t>
+    <t>N9524</t>
+  </si>
+  <si>
+    <t>N9525</t>
   </si>
 </sst>
 </file>
@@ -348,7 +345,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -385,11 +382,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Cambria"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -399,7 +391,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -422,24 +414,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -457,11 +438,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -743,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1267,7 +1244,7 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>75</v>
       </c>
@@ -1283,7 +1260,7 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>76</v>
       </c>
@@ -1299,7 +1276,7 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>77</v>
       </c>
@@ -1315,7 +1292,7 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>78</v>
       </c>
@@ -1331,7 +1308,7 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>79</v>
       </c>
@@ -1347,7 +1324,7 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>80</v>
       </c>
@@ -1363,7 +1340,7 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>81</v>
       </c>
@@ -1379,7 +1356,7 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>82</v>
       </c>
@@ -1393,7 +1370,7 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>83</v>
       </c>
@@ -1407,7 +1384,7 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>84</v>
       </c>
@@ -1420,11 +1397,8 @@
       <c r="F42" s="6">
         <v>42796</v>
       </c>
-      <c r="G42" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>85</v>
       </c>
@@ -1437,11 +1411,8 @@
       <c r="F43" s="6">
         <v>42796</v>
       </c>
-      <c r="G43" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
@@ -1454,11 +1425,8 @@
       <c r="F44" s="6">
         <v>42796</v>
       </c>
-      <c r="G44" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>87</v>
       </c>
@@ -1471,11 +1439,8 @@
       <c r="F45" s="6">
         <v>42796</v>
       </c>
-      <c r="G45" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>88</v>
       </c>
@@ -1488,11 +1453,8 @@
       <c r="F46" s="6">
         <v>42796</v>
       </c>
-      <c r="G46" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>89</v>
       </c>
@@ -1505,11 +1467,8 @@
       <c r="F47" s="6">
         <v>42796</v>
       </c>
-      <c r="G47" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>90</v>
       </c>
@@ -1522,43 +1481,36 @@
       <c r="F48" s="6">
         <v>42796</v>
       </c>
-      <c r="G48" t="s">
+    </row>
+    <row r="49" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F49" s="7">
-        <v>42811</v>
-      </c>
-      <c r="G49" s="8" t="s">
+      <c r="F49" s="6">
+        <v>42817</v>
+      </c>
+      <c r="G49" s="7"/>
+    </row>
+    <row r="50" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F50" s="7">
-        <v>42811</v>
-      </c>
-      <c r="G50" s="8" t="s">
-        <v>100</v>
-      </c>
+      <c r="F50" s="6">
+        <v>42817</v>
+      </c>
+      <c r="G50" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
first build and updated list of WG nb
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_EWH/WG_Number_excel_table.xlsx
+++ b/publication/part1000/CR_EWH/WG_Number_excel_table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10120" yWindow="-19280" windowWidth="28800" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="3160" yWindow="-19280" windowWidth="28800" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WG NB" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="136">
   <si>
     <t>Submitter</t>
   </si>
@@ -336,6 +336,106 @@
   </si>
   <si>
     <t>N9525</t>
+  </si>
+  <si>
+    <t>Kevin Le Tutour</t>
+  </si>
+  <si>
+    <t>pub index wg.number.publication_set_comments</t>
+  </si>
+  <si>
+    <t>CR_EWH project leader check list</t>
+  </si>
+  <si>
+    <t>N9530</t>
+  </si>
+  <si>
+    <t>N9531</t>
+  </si>
+  <si>
+    <t>CR_EWH internal review check list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISO 10303-1828 ed1 wiring_harness_assembly_design Document 
+</t>
+  </si>
+  <si>
+    <t>N9548</t>
+  </si>
+  <si>
+    <t>N9549</t>
+  </si>
+  <si>
+    <t>ISO 10303-1828 ed1 wiring_harness_assembly_design ARM EXPRESS</t>
+  </si>
+  <si>
+    <t>N9550</t>
+  </si>
+  <si>
+    <t>ISO 10303-1828 ed1 wiring_harness_assembly_design MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>N9538</t>
+  </si>
+  <si>
+    <t>CR_EWH project leader check list for new module 1826</t>
+  </si>
+  <si>
+    <t>N9539</t>
+  </si>
+  <si>
+    <t>CR_EWH internal review check list for new module 1826</t>
+  </si>
+  <si>
+    <t>N9540</t>
+  </si>
+  <si>
+    <t>CR_EWH project leader check list for new module 1827</t>
+  </si>
+  <si>
+    <t>N9541</t>
+  </si>
+  <si>
+    <t>CR_EWH internal review check list for new module 1827</t>
+  </si>
+  <si>
+    <t>N9542</t>
+  </si>
+  <si>
+    <t>CR_EWH project leader check list for new module 1828</t>
+  </si>
+  <si>
+    <t>N9543</t>
+  </si>
+  <si>
+    <t>CR_EWH internal review check list for new module 1828</t>
+  </si>
+  <si>
+    <t>N9544</t>
+  </si>
+  <si>
+    <t>R_EWH project leader check list for new module 1844</t>
+  </si>
+  <si>
+    <t>N9545</t>
+  </si>
+  <si>
+    <t>CR_EWH internal review check list for new module 1844</t>
+  </si>
+  <si>
+    <t>N9546</t>
+  </si>
+  <si>
+    <t>CR_EWH project leader check list for new module 1845</t>
+  </si>
+  <si>
+    <t>N9547</t>
+  </si>
+  <si>
+    <t>CR_EWH internal review check list for new module 1845</t>
+  </si>
+  <si>
+    <t>N9474</t>
   </si>
 </sst>
 </file>
@@ -415,8 +515,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -440,9 +542,11 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -718,9 +822,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
@@ -1512,6 +1616,236 @@
       </c>
       <c r="G50" s="7"/>
     </row>
+    <row r="51" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F51" s="6">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F52" s="6">
+        <v>42822</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F53" s="6">
+        <v>42822</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F54" s="6">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F55" s="6">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F56" s="6">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F57" s="6">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F58" s="6">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F59" s="6">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F60" s="6">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F61" s="6">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F62" s="6">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F63" s="6">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F64" s="6">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F65" s="6">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F66" s="6">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
moved 442 to CR_designAPs_1, updated WG N nb table
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_EWH/WG_Number_excel_table.xlsx
+++ b/publication/part1000/CR_EWH/WG_Number_excel_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="-19280" windowWidth="28800" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="-6440" yWindow="-21160" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WG NB" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="130">
   <si>
     <t>Submitter</t>
   </si>
@@ -68,15 +68,6 @@
     <t>ISO 10303-1649 ed4 assembly_technology MIM EXPRESS</t>
   </si>
   <si>
-    <t>ISO 10303-1653 ed4 cable Document</t>
-  </si>
-  <si>
-    <t>ISO 10303-1653 ed4 cable ARM EXPRESS</t>
-  </si>
-  <si>
-    <t>ISO 10303-1653 ed4 cable MIM EXPRESS</t>
-  </si>
-  <si>
     <t>ISO 10303-1657 ed4 component_feature Document</t>
   </si>
   <si>
@@ -186,15 +177,6 @@
   </si>
   <si>
     <t>N9483</t>
-  </si>
-  <si>
-    <t>N9484</t>
-  </si>
-  <si>
-    <t>N9485</t>
-  </si>
-  <si>
-    <t>N9486</t>
   </si>
   <si>
     <t>N9487</t>
@@ -822,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -854,10 +836,10 @@
     </row>
     <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -870,10 +852,10 @@
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -886,10 +868,10 @@
     </row>
     <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -902,10 +884,10 @@
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -918,10 +900,10 @@
     </row>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -934,10 +916,10 @@
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -950,10 +932,10 @@
     </row>
     <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -966,10 +948,10 @@
     </row>
     <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -982,10 +964,10 @@
     </row>
     <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -998,10 +980,10 @@
     </row>
     <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1014,10 +996,10 @@
     </row>
     <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1030,10 +1012,10 @@
     </row>
     <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1046,10 +1028,10 @@
     </row>
     <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1062,10 +1044,10 @@
     </row>
     <row r="15" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1078,10 +1060,10 @@
     </row>
     <row r="16" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1094,10 +1076,10 @@
     </row>
     <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1110,10 +1092,10 @@
     </row>
     <row r="18" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1126,10 +1108,10 @@
     </row>
     <row r="19" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1142,10 +1124,10 @@
     </row>
     <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1158,10 +1140,10 @@
     </row>
     <row r="21" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1174,10 +1156,10 @@
     </row>
     <row r="22" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1190,10 +1172,10 @@
     </row>
     <row r="23" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1206,10 +1188,10 @@
     </row>
     <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1222,10 +1204,10 @@
     </row>
     <row r="25" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1238,10 +1220,10 @@
     </row>
     <row r="26" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1254,10 +1236,10 @@
     </row>
     <row r="27" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1270,10 +1252,10 @@
     </row>
     <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1286,10 +1268,10 @@
     </row>
     <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1302,10 +1284,10 @@
     </row>
     <row r="30" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1318,10 +1300,10 @@
     </row>
     <row r="31" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1334,10 +1316,10 @@
     </row>
     <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1348,12 +1330,12 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1364,12 +1346,12 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1380,12 +1362,12 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1396,12 +1378,12 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1412,15 +1394,13 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+        <v>85</v>
+      </c>
       <c r="E37" s="5" t="s">
         <v>39</v>
       </c>
@@ -1428,15 +1408,13 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+        <v>85</v>
+      </c>
       <c r="E38" s="5" t="s">
         <v>40</v>
       </c>
@@ -1444,240 +1422,238 @@
         <v>42796</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F40" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F43" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F39" s="6">
-        <v>42796</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F40" s="6">
-        <v>42796</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F41" s="6">
-        <v>42796</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="F44" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E42" s="5" t="s">
+      <c r="B45" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F42" s="6">
-        <v>42796</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E43" s="5" t="s">
+      <c r="F45" s="6">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F43" s="6">
-        <v>42796</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E44" s="5" t="s">
+      <c r="F46" s="6">
+        <v>42817</v>
+      </c>
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F44" s="6">
-        <v>42796</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F45" s="6">
-        <v>42796</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F46" s="6">
-        <v>42796</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E47" s="5" t="s">
+      <c r="F47" s="6">
+        <v>42817</v>
+      </c>
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="F47" s="6">
-        <v>42796</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>98</v>
       </c>
       <c r="F48" s="6">
-        <v>42796</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>99</v>
       </c>
       <c r="F49" s="6">
-        <v>42817</v>
-      </c>
-      <c r="G49" s="7"/>
-    </row>
-    <row r="50" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>42822</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="F50" s="6">
-        <v>42817</v>
-      </c>
-      <c r="G50" s="7"/>
-    </row>
-    <row r="51" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>42822</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E51" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E51" s="5" t="s">
-        <v>104</v>
-      </c>
       <c r="F51" s="6">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E52" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="F52" s="6">
-        <v>42822</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>108</v>
       </c>
       <c r="F53" s="6">
-        <v>42822</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>109</v>
       </c>
       <c r="F54" s="6">
         <v>42708</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>112</v>
@@ -1686,12 +1662,12 @@
         <v>42708</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>114</v>
@@ -1700,12 +1676,12 @@
         <v>42708</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>116</v>
@@ -1714,12 +1690,12 @@
         <v>42708</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>117</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>118</v>
@@ -1728,12 +1704,12 @@
         <v>42708</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>120</v>
@@ -1742,12 +1718,12 @@
         <v>42708</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>122</v>
@@ -1756,12 +1732,12 @@
         <v>42708</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>124</v>
@@ -1770,12 +1746,12 @@
         <v>42708</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>126</v>
@@ -1784,12 +1760,12 @@
         <v>42708</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>128</v>
@@ -1798,53 +1774,11 @@
         <v>42708</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F64" s="6">
-        <v>42708</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F65" s="6">
-        <v>42708</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F66" s="6">
-        <v>42708</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="6"/>
+    <row r="64" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
build files used for english review
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_EWH/WG_Number_excel_table.xlsx
+++ b/publication/part1000/CR_EWH/WG_Number_excel_table.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="139">
   <si>
     <t>ISO 10303-1636 ed5 assembly_module_design Document</t>
   </si>
@@ -305,21 +305,6 @@
     <t>Kevin Le Tutour</t>
   </si>
   <si>
-    <t>pub index wg.number.publication_set_comments</t>
-  </si>
-  <si>
-    <t>CR_EWH project leader check list</t>
-  </si>
-  <si>
-    <t>N9530</t>
-  </si>
-  <si>
-    <t>N9531</t>
-  </si>
-  <si>
-    <t>CR_EWH internal review check list</t>
-  </si>
-  <si>
     <t>N9548</t>
   </si>
   <si>
@@ -335,66 +320,6 @@
     <t>ISO 10303-1828 ed1 wiring_harness_assembly_design MIM EXPRESS</t>
   </si>
   <si>
-    <t>N9538</t>
-  </si>
-  <si>
-    <t>CR_EWH project leader check list for new module 1826</t>
-  </si>
-  <si>
-    <t>N9539</t>
-  </si>
-  <si>
-    <t>CR_EWH internal review check list for new module 1826</t>
-  </si>
-  <si>
-    <t>N9540</t>
-  </si>
-  <si>
-    <t>CR_EWH project leader check list for new module 1827</t>
-  </si>
-  <si>
-    <t>N9541</t>
-  </si>
-  <si>
-    <t>CR_EWH internal review check list for new module 1827</t>
-  </si>
-  <si>
-    <t>N9542</t>
-  </si>
-  <si>
-    <t>CR_EWH project leader check list for new module 1828</t>
-  </si>
-  <si>
-    <t>N9543</t>
-  </si>
-  <si>
-    <t>CR_EWH internal review check list for new module 1828</t>
-  </si>
-  <si>
-    <t>N9544</t>
-  </si>
-  <si>
-    <t>N9545</t>
-  </si>
-  <si>
-    <t>CR_EWH internal review check list for new module 1844</t>
-  </si>
-  <si>
-    <t>N9546</t>
-  </si>
-  <si>
-    <t>CR_EWH project leader check list for new module 1845</t>
-  </si>
-  <si>
-    <t>N9547</t>
-  </si>
-  <si>
-    <t>CR_EWH internal review check list for new module 1845</t>
-  </si>
-  <si>
-    <t>N9474</t>
-  </si>
-  <si>
     <t>ISO 10303-1815 ed3 mating_structure Document</t>
   </si>
   <si>
@@ -431,9 +356,6 @@
     <t>ISO 10303-1826 ed1 physical_connectivity_layout_topology_requirement MIM EXPRESS</t>
   </si>
   <si>
-    <t>CR_EWH project leader check list for new module 1844</t>
-  </si>
-  <si>
     <t>ISO 10303-1063 ed4 product_occurrence Document</t>
   </si>
   <si>
@@ -519,6 +441,9 @@
   </si>
   <si>
     <t>ISO 10303-1807 ed2 part_shape MIM EXPRESS</t>
+  </si>
+  <si>
+    <t>N0000</t>
   </si>
 </sst>
 </file>
@@ -935,7 +860,7 @@
   <dimension ref="A1:L82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="93" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61:F63"/>
+      <selection activeCell="F82" sqref="A70:F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -952,44 +877,44 @@
   <sheetData>
     <row r="1" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1758,128 +1683,128 @@
     </row>
     <row r="46" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1926,13 +1851,13 @@
     </row>
     <row r="58" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="F58" s="3">
         <v>42708</v>
@@ -1940,13 +1865,13 @@
     </row>
     <row r="59" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F59" s="3">
         <v>42708</v>
@@ -1954,345 +1879,247 @@
     </row>
     <row r="60" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F60" s="3">
         <v>42708</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="4"/>
+      <c r="A61" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="B61" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="F61" s="4"/>
     </row>
     <row r="62" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="4"/>
+      <c r="A62" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="B62" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="F62" s="4"/>
     </row>
     <row r="63" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="4"/>
+      <c r="A63" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="B63" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="F63" s="4"/>
     </row>
     <row r="64" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B70" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="A70" s="10"/>
+      <c r="B70" s="10"/>
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
-      <c r="E70" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="F70" s="12">
-        <v>2017</v>
-      </c>
+      <c r="E70" s="11"/>
+      <c r="F70" s="12"/>
     </row>
     <row r="71" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B71" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="A71" s="10"/>
+      <c r="B71" s="10"/>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
-      <c r="E71" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F71" s="12">
-        <v>42822</v>
-      </c>
+      <c r="E71" s="11"/>
+      <c r="F71" s="12"/>
     </row>
     <row r="72" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B72" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="A72" s="10"/>
+      <c r="B72" s="10"/>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
-      <c r="E72" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="F72" s="12">
-        <v>42822</v>
-      </c>
+      <c r="E72" s="11"/>
+      <c r="F72" s="12"/>
     </row>
     <row r="73" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B73" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="A73" s="10"/>
+      <c r="B73" s="10"/>
       <c r="C73" s="11"/>
       <c r="D73" s="11"/>
-      <c r="E73" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="F73" s="12">
-        <v>42708</v>
-      </c>
+      <c r="E73" s="11"/>
+      <c r="F73" s="12"/>
     </row>
     <row r="74" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B74" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="A74" s="10"/>
+      <c r="B74" s="10"/>
       <c r="C74" s="11"/>
       <c r="D74" s="11"/>
-      <c r="E74" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F74" s="12">
-        <v>42708</v>
-      </c>
+      <c r="E74" s="11"/>
+      <c r="F74" s="12"/>
     </row>
     <row r="75" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B75" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="A75" s="10"/>
+      <c r="B75" s="10"/>
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
-      <c r="E75" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F75" s="12">
-        <v>42708</v>
-      </c>
+      <c r="E75" s="11"/>
+      <c r="F75" s="12"/>
     </row>
     <row r="76" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B76" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="A76" s="10"/>
+      <c r="B76" s="10"/>
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
-      <c r="E76" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="F76" s="12">
-        <v>42708</v>
-      </c>
+      <c r="E76" s="11"/>
+      <c r="F76" s="12"/>
     </row>
     <row r="77" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B77" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="A77" s="10"/>
+      <c r="B77" s="10"/>
       <c r="C77" s="11"/>
       <c r="D77" s="11"/>
-      <c r="E77" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="F77" s="12">
-        <v>42708</v>
-      </c>
+      <c r="E77" s="11"/>
+      <c r="F77" s="12"/>
     </row>
     <row r="78" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="A78" s="10"/>
+      <c r="B78" s="10"/>
       <c r="C78" s="11"/>
       <c r="D78" s="11"/>
-      <c r="E78" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F78" s="12">
-        <v>42708</v>
-      </c>
+      <c r="E78" s="11"/>
+      <c r="F78" s="12"/>
     </row>
     <row r="79" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B79" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="A79" s="10"/>
+      <c r="B79" s="10"/>
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
-      <c r="E79" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="F79" s="12">
-        <v>42708</v>
-      </c>
+      <c r="E79" s="11"/>
+      <c r="F79" s="12"/>
     </row>
     <row r="80" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B80" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="A80" s="10"/>
+      <c r="B80" s="10"/>
       <c r="C80" s="11"/>
       <c r="D80" s="11"/>
-      <c r="E80" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F80" s="12">
-        <v>42708</v>
-      </c>
+      <c r="E80" s="11"/>
+      <c r="F80" s="12"/>
     </row>
     <row r="81" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B81" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="A81" s="10"/>
+      <c r="B81" s="10"/>
       <c r="C81" s="11"/>
       <c r="D81" s="11"/>
-      <c r="E81" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="F81" s="12">
-        <v>42708</v>
-      </c>
+      <c r="E81" s="11"/>
+      <c r="F81" s="12"/>
     </row>
     <row r="82" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="B82" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="A82" s="10"/>
+      <c r="B82" s="10"/>
       <c r="C82" s="11"/>
       <c r="D82" s="11"/>
-      <c r="E82" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="F82" s="12">
-        <v>42708</v>
-      </c>
+      <c r="E82" s="11"/>
+      <c r="F82" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Completed with missing N number, change edition number for some parts which were already in a previous CR of 242e2
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_EWH/WG_Number_excel_table.xlsx
+++ b/publication/part1000/CR_EWH/WG_Number_excel_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10380" yWindow="-21160" windowWidth="21580" windowHeight="20480" tabRatio="500"/>
+    <workbookView xWindow="-6440" yWindow="-21600" windowWidth="19140" windowHeight="20280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WG NB" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="167">
   <si>
     <t>ISO 10303-1636 ed5 assembly_module_design Document</t>
   </si>
@@ -305,6 +305,21 @@
     <t>Kevin Le Tutour</t>
   </si>
   <si>
+    <t>pub index wg.number.publication_set_comments</t>
+  </si>
+  <si>
+    <t>CR_EWH project leader check list</t>
+  </si>
+  <si>
+    <t>N9530</t>
+  </si>
+  <si>
+    <t>N9531</t>
+  </si>
+  <si>
+    <t>CR_EWH internal review check list</t>
+  </si>
+  <si>
     <t>N9548</t>
   </si>
   <si>
@@ -320,6 +335,66 @@
     <t>ISO 10303-1828 ed1 wiring_harness_assembly_design MIM EXPRESS</t>
   </si>
   <si>
+    <t>N9538</t>
+  </si>
+  <si>
+    <t>CR_EWH project leader check list for new module 1826</t>
+  </si>
+  <si>
+    <t>N9539</t>
+  </si>
+  <si>
+    <t>CR_EWH internal review check list for new module 1826</t>
+  </si>
+  <si>
+    <t>N9540</t>
+  </si>
+  <si>
+    <t>CR_EWH project leader check list for new module 1827</t>
+  </si>
+  <si>
+    <t>N9541</t>
+  </si>
+  <si>
+    <t>CR_EWH internal review check list for new module 1827</t>
+  </si>
+  <si>
+    <t>N9542</t>
+  </si>
+  <si>
+    <t>CR_EWH project leader check list for new module 1828</t>
+  </si>
+  <si>
+    <t>N9543</t>
+  </si>
+  <si>
+    <t>CR_EWH internal review check list for new module 1828</t>
+  </si>
+  <si>
+    <t>N9544</t>
+  </si>
+  <si>
+    <t>N9545</t>
+  </si>
+  <si>
+    <t>CR_EWH internal review check list for new module 1844</t>
+  </si>
+  <si>
+    <t>N9546</t>
+  </si>
+  <si>
+    <t>CR_EWH project leader check list for new module 1845</t>
+  </si>
+  <si>
+    <t>N9547</t>
+  </si>
+  <si>
+    <t>CR_EWH internal review check list for new module 1845</t>
+  </si>
+  <si>
+    <t>N9474</t>
+  </si>
+  <si>
     <t>ISO 10303-1815 ed3 mating_structure Document</t>
   </si>
   <si>
@@ -356,6 +431,9 @@
     <t>ISO 10303-1826 ed1 physical_connectivity_layout_topology_requirement MIM EXPRESS</t>
   </si>
   <si>
+    <t>CR_EWH project leader check list for new module 1844</t>
+  </si>
+  <si>
     <t>ISO 10303-1063 ed4 product_occurrence Document</t>
   </si>
   <si>
@@ -443,7 +521,13 @@
     <t>ISO 10303-1807 ed2 part_shape MIM EXPRESS</t>
   </si>
   <si>
-    <t>N0000</t>
+    <t>N9706</t>
+  </si>
+  <si>
+    <t>N9707</t>
+  </si>
+  <si>
+    <t>N9708</t>
   </si>
 </sst>
 </file>
@@ -491,8 +575,8 @@
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Cambria"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -536,18 +620,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -562,16 +640,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -859,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="93" workbookViewId="0">
-      <selection activeCell="F82" sqref="A70:F82"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="93" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -870,51 +951,51 @@
     <col min="3" max="4" width="10.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="98.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" style="1" customWidth="1"/>
-    <col min="7" max="10" width="10.83203125" style="7"/>
-    <col min="11" max="11" width="117.1640625" style="7" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="7"/>
+    <col min="7" max="10" width="10.83203125" style="5"/>
+    <col min="11" max="11" width="117.1640625" style="5" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>113</v>
+      <c r="E1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>113</v>
+      <c r="E2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>113</v>
+      <c r="E3" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -926,10 +1007,10 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -942,10 +1023,10 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -958,10 +1039,10 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -974,18 +1055,18 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
+      <c r="F7" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -996,18 +1077,18 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
+      <c r="F8" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -1018,18 +1099,18 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
+      <c r="F9" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -1040,18 +1121,18 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
+      <c r="F10" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -1062,18 +1143,18 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
+      <c r="F11" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -1084,18 +1165,18 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
+      <c r="F12" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -1106,18 +1187,18 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
+      <c r="F13" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -1128,18 +1209,18 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
+      <c r="F14" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -1150,18 +1231,18 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
+      <c r="F15" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -1172,18 +1253,18 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
+      <c r="F16" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
     </row>
     <row r="17" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -1194,18 +1275,18 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
+      <c r="F17" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
     </row>
     <row r="18" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -1216,18 +1297,18 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
+      <c r="F18" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
@@ -1238,18 +1319,18 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
+      <c r="F19" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
     </row>
     <row r="20" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
@@ -1260,18 +1341,18 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
+      <c r="F20" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
     </row>
     <row r="21" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -1282,18 +1363,18 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
+      <c r="F21" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
     </row>
     <row r="22" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -1304,18 +1385,18 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
+      <c r="F22" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
     </row>
     <row r="23" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
@@ -1326,18 +1407,18 @@
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
+      <c r="F23" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
     </row>
     <row r="24" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
@@ -1348,18 +1429,18 @@
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="3">
-        <v>42796</v>
-      </c>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
+      <c r="F24" s="9">
+        <v>42796</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
     </row>
     <row r="25" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
@@ -1370,10 +1451,10 @@
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1386,10 +1467,10 @@
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1402,10 +1483,10 @@
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1418,10 +1499,10 @@
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1434,10 +1515,10 @@
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1450,10 +1531,10 @@
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1466,10 +1547,10 @@
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1482,10 +1563,10 @@
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1498,10 +1579,10 @@
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1514,10 +1595,10 @@
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1530,10 +1611,10 @@
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1546,10 +1627,10 @@
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1562,10 +1643,10 @@
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1576,10 +1657,10 @@
       <c r="B38" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1590,10 +1671,10 @@
       <c r="B39" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1601,13 +1682,13 @@
       <c r="A40" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E40" s="1" t="s">
+      <c r="B40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1615,13 +1696,13 @@
       <c r="A41" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="B41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1629,13 +1710,13 @@
       <c r="A42" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E42" s="1" t="s">
+      <c r="B42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1643,13 +1724,13 @@
       <c r="A43" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E43" s="1" t="s">
+      <c r="B43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1657,13 +1738,13 @@
       <c r="A44" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E44" s="1" t="s">
+      <c r="B44" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44" s="9">
         <v>42796</v>
       </c>
     </row>
@@ -1671,455 +1752,539 @@
       <c r="A45" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E45" s="1" t="s">
+      <c r="B45" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45" s="9">
         <v>42796</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F46" s="9" t="s">
-        <v>113</v>
+      <c r="E46" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="F46" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>113</v>
+      <c r="E47" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="F47" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>113</v>
+      <c r="E48" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F48" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F49" s="9" t="s">
-        <v>113</v>
+      <c r="E49" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F49" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>113</v>
+      <c r="E50" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F50" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>113</v>
+      <c r="E51" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F51" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F52" s="9" t="s">
-        <v>113</v>
+      <c r="E52" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>113</v>
+      <c r="E53" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>113</v>
+      <c r="E54" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E55" s="1" t="s">
+      <c r="B55" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E55" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="F55" s="3">
-        <v>42796</v>
+      <c r="F55" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E56" s="1" t="s">
+      <c r="B56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E56" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F56" s="3">
-        <v>42817</v>
+      <c r="F56" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E57" s="1" t="s">
+      <c r="B57" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E57" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F57" s="3">
-        <v>42817</v>
+      <c r="F57" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F58" s="3">
-        <v>42708</v>
+      <c r="E58" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F58" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F59" s="3">
-        <v>42708</v>
+      <c r="E59" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F59" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F60" s="3">
-        <v>42708</v>
+      <c r="E60" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F60" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F61" s="4"/>
+      <c r="A61" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F61" s="8">
+        <v>42548</v>
+      </c>
     </row>
     <row r="62" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="F62" s="4"/>
+      <c r="A62" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="F62" s="8">
+        <v>42548</v>
+      </c>
     </row>
     <row r="63" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F63" s="4"/>
+      <c r="A63" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F63" s="8">
+        <v>42548</v>
+      </c>
     </row>
     <row r="64" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F64" s="9" t="s">
-        <v>113</v>
+      <c r="E64" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F64" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F65" s="9" t="s">
-        <v>113</v>
+      <c r="E65" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F65" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E66" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>113</v>
+      <c r="E66" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F66" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>113</v>
+      <c r="E67" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F67" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F68" s="9" t="s">
-        <v>113</v>
+      <c r="E68" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F68" s="8">
+        <v>42548</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E69" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F69" s="8">
+        <v>42548</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F70" s="9">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F71" s="9">
+        <v>42822</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F72" s="9">
+        <v>42822</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F73" s="9">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F74" s="9">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F69" s="9" t="s">
+      <c r="B75" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F75" s="9">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F76" s="9">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F77" s="9">
+        <v>42708</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E78" s="7" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="10"/>
-      <c r="B70" s="10"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="12"/>
-    </row>
-    <row r="71" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="10"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="12"/>
-    </row>
-    <row r="72" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="10"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="11"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
-      <c r="F72" s="12"/>
-    </row>
-    <row r="73" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="10"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="12"/>
-    </row>
-    <row r="74" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="10"/>
-      <c r="B74" s="10"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="12"/>
-    </row>
-    <row r="75" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="10"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
-      <c r="F75" s="12"/>
-    </row>
-    <row r="76" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="10"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="12"/>
-    </row>
-    <row r="77" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="10"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="12"/>
-    </row>
-    <row r="78" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="10"/>
-      <c r="B78" s="10"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="12"/>
+      <c r="F78" s="9">
+        <v>42708</v>
+      </c>
     </row>
     <row r="79" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="10"/>
-      <c r="B79" s="10"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="12"/>
+      <c r="A79" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F79" s="9">
+        <v>42708</v>
+      </c>
     </row>
     <row r="80" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="10"/>
-      <c r="B80" s="10"/>
-      <c r="C80" s="11"/>
-      <c r="D80" s="11"/>
-      <c r="E80" s="11"/>
-      <c r="F80" s="12"/>
+      <c r="A80" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F80" s="9">
+        <v>42708</v>
+      </c>
     </row>
     <row r="81" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="10"/>
-      <c r="B81" s="10"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
-      <c r="F81" s="12"/>
+      <c r="A81" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F81" s="9">
+        <v>42708</v>
+      </c>
     </row>
     <row r="82" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="10"/>
-      <c r="B82" s="10"/>
-      <c r="C82" s="11"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="12"/>
+      <c r="A82" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F82" s="9">
+        <v>42708</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>